<commit_message>
commit view for account. only index and list Signed-off-by: locdv <dinhvanloc25@gmail.com>
</commit_message>
<xml_diff>
--- a/Datatest/Account.xlsx
+++ b/Datatest/Account.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\MyCrm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\MyCrm\CloneCrm\Datatest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
-  <si>
-    <t>id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -44,12 +41,6 @@
     <t>shipping address</t>
   </si>
   <si>
-    <t>created by</t>
-  </si>
-  <si>
-    <t>created on</t>
-  </si>
-  <si>
     <t xml:space="preserve"> website</t>
   </si>
   <si>
@@ -74,9 +65,6 @@
     <t xml:space="preserve">AGRICULTURE </t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t xml:space="preserve">HEALTHCARE </t>
   </si>
   <si>
@@ -92,9 +80,6 @@
     <t>Billing adress</t>
   </si>
   <si>
-    <t>Descript</t>
-  </si>
-  <si>
     <t>Assigned to</t>
   </si>
   <si>
@@ -141,15 +126,15 @@
   </si>
   <si>
     <t>Hoa</t>
+  </si>
+  <si>
+    <t>stt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -185,10 +170,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -470,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,59 +471,47 @@
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="16" customWidth="1"/>
     <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>9</v>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C2" t="str">
         <f>B2&amp;"@gmail.com"</f>
@@ -549,36 +521,27 @@
         <v>973394485</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="2">
-        <v>43473</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C8" si="0">B3&amp;"@gmail.com"</f>
@@ -588,36 +551,27 @@
         <v>973394486</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M3" s="2">
-        <v>43473</v>
-      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -627,36 +581,27 @@
         <v>973394487</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="2">
-        <v>43471</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>36</v>
+      <c r="B5" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -666,36 +611,27 @@
         <v>973394488</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="2">
-        <v>43468</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -705,36 +641,27 @@
         <v>973394489</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M6" s="2">
-        <v>43467</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>37</v>
+      <c r="B7" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -744,36 +671,27 @@
         <v>973394490</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="2">
-        <v>43470</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>38</v>
+      <c r="B8" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -783,32 +701,20 @@
         <v>973394491</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J8" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L8" t="s">
-        <v>25</v>
-      </c>
-      <c r="M8" s="2">
-        <v>43472</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="M9" s="2"/>
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Signed-off-by: locdv <dinhvanloc25@gmail.com> tao list for leads/views.py
</commit_message>
<xml_diff>
--- a/Datatest/Account.xlsx
+++ b/Datatest/Account.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -129,6 +129,159 @@
   </si>
   <si>
     <t>stt</t>
+  </si>
+  <si>
+    <t>Hoa1</t>
+  </si>
+  <si>
+    <t>Hoa2</t>
+  </si>
+  <si>
+    <t>Hoa3</t>
+  </si>
+  <si>
+    <t>Hoa4</t>
+  </si>
+  <si>
+    <t>Hoa5</t>
+  </si>
+  <si>
+    <t>Hoa6</t>
+  </si>
+  <si>
+    <t>Hoa7</t>
+  </si>
+  <si>
+    <t>Hoa8</t>
+  </si>
+  <si>
+    <t>Hoa9</t>
+  </si>
+  <si>
+    <t>Hoa10</t>
+  </si>
+  <si>
+    <t>Hoa11</t>
+  </si>
+  <si>
+    <t>Hoa12</t>
+  </si>
+  <si>
+    <t>Hoa13</t>
+  </si>
+  <si>
+    <t>Hoa14</t>
+  </si>
+  <si>
+    <t>Hoa15</t>
+  </si>
+  <si>
+    <t>Hoa16</t>
+  </si>
+  <si>
+    <t>Hoa17</t>
+  </si>
+  <si>
+    <t>Hoa18</t>
+  </si>
+  <si>
+    <t>Hoa19</t>
+  </si>
+  <si>
+    <t>Hoa20</t>
+  </si>
+  <si>
+    <t>Hoa21</t>
+  </si>
+  <si>
+    <t>Hoa22</t>
+  </si>
+  <si>
+    <t>Hoa23</t>
+  </si>
+  <si>
+    <t>Hoa24</t>
+  </si>
+  <si>
+    <t>Hoa25</t>
+  </si>
+  <si>
+    <t>Hoa26</t>
+  </si>
+  <si>
+    <t>Hoa27</t>
+  </si>
+  <si>
+    <t>Hoa28</t>
+  </si>
+  <si>
+    <t>Hoa29</t>
+  </si>
+  <si>
+    <t>Hoa30</t>
+  </si>
+  <si>
+    <t>Hoa31</t>
+  </si>
+  <si>
+    <t>Hoa32</t>
+  </si>
+  <si>
+    <t>Hoa33</t>
+  </si>
+  <si>
+    <t>Hoa34</t>
+  </si>
+  <si>
+    <t>Hoa35</t>
+  </si>
+  <si>
+    <t>Hoa36</t>
+  </si>
+  <si>
+    <t>Hoa37</t>
+  </si>
+  <si>
+    <t>Hoa38</t>
+  </si>
+  <si>
+    <t>Hoa39</t>
+  </si>
+  <si>
+    <t>Hoa40</t>
+  </si>
+  <si>
+    <t>Hoa41</t>
+  </si>
+  <si>
+    <t>Hoa42</t>
+  </si>
+  <si>
+    <t>Hoa43</t>
+  </si>
+  <si>
+    <t>Hoa44</t>
+  </si>
+  <si>
+    <t>Hoa45</t>
+  </si>
+  <si>
+    <t>Hoa46</t>
+  </si>
+  <si>
+    <t>Hoa47</t>
+  </si>
+  <si>
+    <t>Hoa48</t>
+  </si>
+  <si>
+    <t>Hoa49</t>
+  </si>
+  <si>
+    <t>Hoa50</t>
+  </si>
+  <si>
+    <t>Hoa51</t>
   </si>
 </sst>
 </file>
@@ -454,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,6 +869,1536 @@
         <v>16</v>
       </c>
     </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" ref="C9" si="1">B9&amp;"@gmail.com"</f>
+        <v>Hoa1@gmail.com</v>
+      </c>
+      <c r="D9">
+        <v>973394492</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" ref="C10:C59" si="2">B10&amp;"@gmail.com"</f>
+        <v>Hoa2@gmail.com</v>
+      </c>
+      <c r="D10">
+        <v>973394493</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa3@gmail.com</v>
+      </c>
+      <c r="D11">
+        <v>973394494</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa4@gmail.com</v>
+      </c>
+      <c r="D12">
+        <v>973394495</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa5@gmail.com</v>
+      </c>
+      <c r="D13">
+        <v>973394496</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa6@gmail.com</v>
+      </c>
+      <c r="D14">
+        <v>973394497</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa7@gmail.com</v>
+      </c>
+      <c r="D15">
+        <v>973394498</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa8@gmail.com</v>
+      </c>
+      <c r="D16">
+        <v>973394499</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa9@gmail.com</v>
+      </c>
+      <c r="D17">
+        <v>973394500</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa10@gmail.com</v>
+      </c>
+      <c r="D18">
+        <v>973394501</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa11@gmail.com</v>
+      </c>
+      <c r="D19">
+        <v>973394502</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa12@gmail.com</v>
+      </c>
+      <c r="D20">
+        <v>973394503</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa13@gmail.com</v>
+      </c>
+      <c r="D21">
+        <v>973394504</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa14@gmail.com</v>
+      </c>
+      <c r="D22">
+        <v>973394505</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa15@gmail.com</v>
+      </c>
+      <c r="D23">
+        <v>973394506</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa16@gmail.com</v>
+      </c>
+      <c r="D24">
+        <v>973394507</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" t="s">
+        <v>30</v>
+      </c>
+      <c r="H24" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa17@gmail.com</v>
+      </c>
+      <c r="D25">
+        <v>973394508</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" t="s">
+        <v>21</v>
+      </c>
+      <c r="J25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa18@gmail.com</v>
+      </c>
+      <c r="D26">
+        <v>973394509</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa19@gmail.com</v>
+      </c>
+      <c r="D27">
+        <v>973394510</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" t="s">
+        <v>30</v>
+      </c>
+      <c r="H27" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa20@gmail.com</v>
+      </c>
+      <c r="D28">
+        <v>973394511</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" t="s">
+        <v>21</v>
+      </c>
+      <c r="J28" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa21@gmail.com</v>
+      </c>
+      <c r="D29">
+        <v>973394512</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" t="s">
+        <v>30</v>
+      </c>
+      <c r="H29" t="s">
+        <v>21</v>
+      </c>
+      <c r="J29" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa22@gmail.com</v>
+      </c>
+      <c r="D30">
+        <v>973394513</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30" t="s">
+        <v>30</v>
+      </c>
+      <c r="H30" t="s">
+        <v>21</v>
+      </c>
+      <c r="J30" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa23@gmail.com</v>
+      </c>
+      <c r="D31">
+        <v>973394514</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" t="s">
+        <v>21</v>
+      </c>
+      <c r="J31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa24@gmail.com</v>
+      </c>
+      <c r="D32">
+        <v>973394515</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32" t="s">
+        <v>21</v>
+      </c>
+      <c r="J32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa25@gmail.com</v>
+      </c>
+      <c r="D33">
+        <v>973394516</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" t="s">
+        <v>28</v>
+      </c>
+      <c r="G33" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33" t="s">
+        <v>21</v>
+      </c>
+      <c r="J33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa26@gmail.com</v>
+      </c>
+      <c r="D34">
+        <v>973394517</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" t="s">
+        <v>28</v>
+      </c>
+      <c r="G34" t="s">
+        <v>30</v>
+      </c>
+      <c r="H34" t="s">
+        <v>21</v>
+      </c>
+      <c r="J34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa27@gmail.com</v>
+      </c>
+      <c r="D35">
+        <v>973394518</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" t="s">
+        <v>28</v>
+      </c>
+      <c r="G35" t="s">
+        <v>30</v>
+      </c>
+      <c r="H35" t="s">
+        <v>21</v>
+      </c>
+      <c r="J35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa28@gmail.com</v>
+      </c>
+      <c r="D36">
+        <v>973394519</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" t="s">
+        <v>28</v>
+      </c>
+      <c r="G36" t="s">
+        <v>30</v>
+      </c>
+      <c r="H36" t="s">
+        <v>21</v>
+      </c>
+      <c r="J36" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa29@gmail.com</v>
+      </c>
+      <c r="D37">
+        <v>973394520</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" t="s">
+        <v>28</v>
+      </c>
+      <c r="G37" t="s">
+        <v>30</v>
+      </c>
+      <c r="H37" t="s">
+        <v>21</v>
+      </c>
+      <c r="J37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa30@gmail.com</v>
+      </c>
+      <c r="D38">
+        <v>973394521</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" t="s">
+        <v>21</v>
+      </c>
+      <c r="J38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa31@gmail.com</v>
+      </c>
+      <c r="D39">
+        <v>973394522</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" t="s">
+        <v>21</v>
+      </c>
+      <c r="J39" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa32@gmail.com</v>
+      </c>
+      <c r="D40">
+        <v>973394523</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" t="s">
+        <v>21</v>
+      </c>
+      <c r="J40" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa33@gmail.com</v>
+      </c>
+      <c r="D41">
+        <v>973394524</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" t="s">
+        <v>21</v>
+      </c>
+      <c r="J41" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa34@gmail.com</v>
+      </c>
+      <c r="D42">
+        <v>973394525</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" t="s">
+        <v>28</v>
+      </c>
+      <c r="G42" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" t="s">
+        <v>21</v>
+      </c>
+      <c r="J42" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa35@gmail.com</v>
+      </c>
+      <c r="D43">
+        <v>973394526</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" t="s">
+        <v>30</v>
+      </c>
+      <c r="H43" t="s">
+        <v>21</v>
+      </c>
+      <c r="J43" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa36@gmail.com</v>
+      </c>
+      <c r="D44">
+        <v>973394527</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" t="s">
+        <v>28</v>
+      </c>
+      <c r="G44" t="s">
+        <v>30</v>
+      </c>
+      <c r="H44" t="s">
+        <v>21</v>
+      </c>
+      <c r="J44" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa37@gmail.com</v>
+      </c>
+      <c r="D45">
+        <v>973394528</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" t="s">
+        <v>28</v>
+      </c>
+      <c r="G45" t="s">
+        <v>30</v>
+      </c>
+      <c r="H45" t="s">
+        <v>21</v>
+      </c>
+      <c r="J45" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa38@gmail.com</v>
+      </c>
+      <c r="D46">
+        <v>973394529</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" t="s">
+        <v>28</v>
+      </c>
+      <c r="G46" t="s">
+        <v>30</v>
+      </c>
+      <c r="H46" t="s">
+        <v>21</v>
+      </c>
+      <c r="J46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa39@gmail.com</v>
+      </c>
+      <c r="D47">
+        <v>973394530</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" t="s">
+        <v>28</v>
+      </c>
+      <c r="G47" t="s">
+        <v>30</v>
+      </c>
+      <c r="H47" t="s">
+        <v>21</v>
+      </c>
+      <c r="J47" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa40@gmail.com</v>
+      </c>
+      <c r="D48">
+        <v>973394531</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" t="s">
+        <v>28</v>
+      </c>
+      <c r="G48" t="s">
+        <v>30</v>
+      </c>
+      <c r="H48" t="s">
+        <v>21</v>
+      </c>
+      <c r="J48" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa41@gmail.com</v>
+      </c>
+      <c r="D49">
+        <v>973394532</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" t="s">
+        <v>28</v>
+      </c>
+      <c r="G49" t="s">
+        <v>30</v>
+      </c>
+      <c r="H49" t="s">
+        <v>21</v>
+      </c>
+      <c r="J49" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa42@gmail.com</v>
+      </c>
+      <c r="D50">
+        <v>973394533</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" t="s">
+        <v>28</v>
+      </c>
+      <c r="G50" t="s">
+        <v>30</v>
+      </c>
+      <c r="H50" t="s">
+        <v>21</v>
+      </c>
+      <c r="J50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa43@gmail.com</v>
+      </c>
+      <c r="D51">
+        <v>973394534</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51" t="s">
+        <v>28</v>
+      </c>
+      <c r="G51" t="s">
+        <v>30</v>
+      </c>
+      <c r="H51" t="s">
+        <v>21</v>
+      </c>
+      <c r="J51" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa44@gmail.com</v>
+      </c>
+      <c r="D52">
+        <v>973394535</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52" t="s">
+        <v>28</v>
+      </c>
+      <c r="G52" t="s">
+        <v>30</v>
+      </c>
+      <c r="H52" t="s">
+        <v>21</v>
+      </c>
+      <c r="J52" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa45@gmail.com</v>
+      </c>
+      <c r="D53">
+        <v>973394536</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F53" t="s">
+        <v>28</v>
+      </c>
+      <c r="G53" t="s">
+        <v>30</v>
+      </c>
+      <c r="H53" t="s">
+        <v>21</v>
+      </c>
+      <c r="J53" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa46@gmail.com</v>
+      </c>
+      <c r="D54">
+        <v>973394537</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" t="s">
+        <v>28</v>
+      </c>
+      <c r="G54" t="s">
+        <v>30</v>
+      </c>
+      <c r="H54" t="s">
+        <v>21</v>
+      </c>
+      <c r="J54" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa47@gmail.com</v>
+      </c>
+      <c r="D55">
+        <v>973394538</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" t="s">
+        <v>28</v>
+      </c>
+      <c r="G55" t="s">
+        <v>30</v>
+      </c>
+      <c r="H55" t="s">
+        <v>21</v>
+      </c>
+      <c r="J55" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa48@gmail.com</v>
+      </c>
+      <c r="D56">
+        <v>973394539</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F56" t="s">
+        <v>28</v>
+      </c>
+      <c r="G56" t="s">
+        <v>30</v>
+      </c>
+      <c r="H56" t="s">
+        <v>21</v>
+      </c>
+      <c r="J56" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa49@gmail.com</v>
+      </c>
+      <c r="D57">
+        <v>973394540</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F57" t="s">
+        <v>28</v>
+      </c>
+      <c r="G57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H57" t="s">
+        <v>21</v>
+      </c>
+      <c r="J57" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa50@gmail.com</v>
+      </c>
+      <c r="D58">
+        <v>973394541</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F58" t="s">
+        <v>28</v>
+      </c>
+      <c r="G58" t="s">
+        <v>30</v>
+      </c>
+      <c r="H58" t="s">
+        <v>21</v>
+      </c>
+      <c r="J58" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="2"/>
+        <v>Hoa51@gmail.com</v>
+      </c>
+      <c r="D59">
+        <v>973394542</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F59" t="s">
+        <v>28</v>
+      </c>
+      <c r="G59" t="s">
+        <v>30</v>
+      </c>
+      <c r="H59" t="s">
+        <v>21</v>
+      </c>
+      <c r="J59" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" horizontalDpi="72" verticalDpi="72" r:id="rId1"/>

</xml_diff>